<commit_message>
Changed min order on cheap components to 10
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MatthewPoole\Documents\Post-Grad\Stanford\MS Aero-Astro\AA236B\PandaSat\electrical-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DB680F-82C7-40F1-B32C-0C0C6604698A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C08B1-01D8-473F-AFB9-2E049F0C78FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{7969AC2C-1119-489B-B180-70BBFC48BFE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7969AC2C-1119-489B-B180-70BBFC48BFE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-S6C" sheetId="1" r:id="rId1"/>
@@ -1489,7 +1489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3A4314-0F82-4785-B06F-435A11FFC277}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1914,7 +1914,7 @@
         <v>79</v>
       </c>
       <c r="D18" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>325</v>
@@ -2466,7 +2466,7 @@
         <v>159</v>
       </c>
       <c r="D43" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>173</v>
@@ -2518,7 +2518,7 @@
         <v>159</v>
       </c>
       <c r="D45" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>170</v>
@@ -2570,7 +2570,7 @@
         <v>159</v>
       </c>
       <c r="D47" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>179</v>
@@ -2596,7 +2596,7 @@
         <v>159</v>
       </c>
       <c r="D48" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>182</v>
@@ -2648,7 +2648,7 @@
         <v>159</v>
       </c>
       <c r="D50" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>188</v>
@@ -2712,7 +2712,7 @@
         <v>159</v>
       </c>
       <c r="D53" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>228</v>
@@ -2738,7 +2738,7 @@
         <v>159</v>
       </c>
       <c r="D54" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>231</v>
@@ -2790,7 +2790,7 @@
         <v>159</v>
       </c>
       <c r="D56" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>312</v>
@@ -2819,7 +2819,7 @@
         <v>159</v>
       </c>
       <c r="D57" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>237</v>
@@ -2871,7 +2871,7 @@
         <v>159</v>
       </c>
       <c r="D59" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>243</v>
@@ -2923,7 +2923,7 @@
         <v>159</v>
       </c>
       <c r="D61" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>249</v>
@@ -2949,7 +2949,7 @@
         <v>159</v>
       </c>
       <c r="D62" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>252</v>
@@ -2975,7 +2975,7 @@
         <v>159</v>
       </c>
       <c r="D63" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>255</v>
@@ -3001,7 +3001,7 @@
         <v>159</v>
       </c>
       <c r="D64" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>317</v>
@@ -3056,7 +3056,7 @@
         <v>159</v>
       </c>
       <c r="D66" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>262</v>
@@ -3082,7 +3082,7 @@
         <v>220</v>
       </c>
       <c r="D67" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>271</v>
@@ -3108,7 +3108,7 @@
         <v>159</v>
       </c>
       <c r="D68" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>265</v>
@@ -3134,7 +3134,7 @@
         <v>159</v>
       </c>
       <c r="D69" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>268</v>
@@ -3151,17 +3151,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A52:H52"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated 'Order' to match BOM
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MatthewPoole\Documents\Post-Grad\Stanford\MS Aero-Astro\AA236B\PandaSat\electrical-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C08B1-01D8-473F-AFB9-2E049F0C78FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E067441-A1FA-4F86-B74D-FEE203A522C0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7969AC2C-1119-489B-B180-70BBFC48BFE9}"/>
   </bookViews>
@@ -605,15 +605,6 @@
     <t>https://www.digikey.com/product-detail/en/kemet/C0603C220J8GAC7867/399-15378-1-ND/7386776</t>
   </si>
   <si>
-    <t>445-6007-1-ND</t>
-  </si>
-  <si>
-    <t>C3216X5R1A107M160AC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/tdk-corporation/C3216X5R1A107M160AC/445-6007-1-ND/2444048</t>
-  </si>
-  <si>
     <t>43K SMD</t>
   </si>
   <si>
@@ -1014,6 +1005,15 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/ON-Semiconductor/BC846BLT1G?qs=sGAEpiMZZMtqO%252bWUGLBzePo0Ry%252bsrgua</t>
+  </si>
+  <si>
+    <t>490-9966-1ND</t>
+  </si>
+  <si>
+    <t>GRM31CE70G107ME39L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM31CE70G107ME39L/490-9966-1-ND/5026462</t>
   </si>
 </sst>
 </file>
@@ -1489,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3A4314-0F82-4785-B06F-435A11FFC277}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,13 +1607,13 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>29</v>
@@ -1633,13 +1633,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>29</v>
@@ -1763,13 +1763,13 @@
         <v>3</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>29</v>
@@ -1865,13 +1865,13 @@
         <v>12</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>29</v>
@@ -1900,7 +1900,7 @@
         <v>76</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1917,16 +1917,16 @@
         <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1964,7 +1964,7 @@
         <v>86</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2028,7 +2028,7 @@
         <v>94</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2066,7 +2066,7 @@
         <v>113</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2074,7 +2074,7 @@
         <v>102</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>118</v>
@@ -2092,7 +2092,7 @@
         <v>115</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2103,22 +2103,22 @@
         <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D27" s="3">
         <v>3</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2144,7 +2144,7 @@
         <v>121</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
         <v>124</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2196,15 +2196,15 @@
         <v>127</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>119</v>
@@ -2213,16 +2213,16 @@
         <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2239,10 +2239,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C33" s="2">
         <v>1210</v>
@@ -2251,24 +2251,24 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C34" s="2">
         <v>1210</v>
@@ -2277,24 +2277,24 @@
         <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C35" s="2">
         <v>1210</v>
@@ -2303,16 +2303,16 @@
         <v>3</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2329,28 +2329,28 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D37" s="3">
         <v>3</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2370,7 +2370,7 @@
         <v>134</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>119</v>
@@ -2388,7 +2388,7 @@
         <v>131</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
         <v>177</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2452,7 +2452,7 @@
         <v>176</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2478,7 +2478,7 @@
         <v>174</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2504,7 +2504,7 @@
         <v>172</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2530,7 +2530,7 @@
         <v>166</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2556,7 +2556,7 @@
         <v>169</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>181</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
         <v>184</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2634,7 +2634,7 @@
         <v>187</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2660,7 +2660,7 @@
         <v>190</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2677,16 +2677,16 @@
         <v>15</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>191</v>
+        <v>325</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>192</v>
+        <v>326</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>193</v>
+        <v>327</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2703,10 +2703,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>159</v>
@@ -2715,24 +2715,24 @@
         <v>10</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>159</v>
@@ -2741,24 +2741,24 @@
         <v>10</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>159</v>
@@ -2767,24 +2767,24 @@
         <v>18</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>159</v>
@@ -2793,27 +2793,27 @@
         <v>10</v>
       </c>
       <c r="E56" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="I56" s="7" t="s">
         <v>312</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>159</v>
@@ -2822,24 +2822,24 @@
         <v>10</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>159</v>
@@ -2848,24 +2848,24 @@
         <v>18</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>159</v>
@@ -2874,24 +2874,24 @@
         <v>10</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>159</v>
@@ -2900,24 +2900,24 @@
         <v>27</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>159</v>
@@ -2926,24 +2926,24 @@
         <v>10</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>159</v>
@@ -2952,24 +2952,24 @@
         <v>10</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>159</v>
@@ -2978,24 +2978,24 @@
         <v>10</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>159</v>
@@ -3004,27 +3004,27 @@
         <v>10</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>159</v>
@@ -3033,24 +3033,24 @@
         <v>15</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>159</v>
@@ -3059,50 +3059,50 @@
         <v>10</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D67" s="3">
         <v>10</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>159</v>
@@ -3111,24 +3111,24 @@
         <v>10</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>159</v>
@@ -3137,31 +3137,31 @@
         <v>10</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A52:H52"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>